<commit_message>
acrescimo da emissao CIN
</commit_message>
<xml_diff>
--- a/Evento_Acoes_Sociais.xlsx
+++ b/Evento_Acoes_Sociais.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Data</t>
   </si>
@@ -139,6 +139,42 @@
   </si>
   <si>
     <t xml:space="preserve">Professor Alves da Silva</t>
+  </si>
+  <si>
+    <t>09:00-16:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vagas - Auxiliar de Logística - Auxilia de Armazém </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JM Empilhadeira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vagas - Telemarketing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolve Já </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vagas - 7 vagas de vendedor(a) ótica/2 recepcionista para cliente/2 Gerentes de vendas (ótica)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Líderes Consultoria e Treinamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vagas - Vendedor Interno /Vendedor externo /Estágio ( Setor Financeiro)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grau Técnico</t>
+  </si>
+  <si>
+    <t>08:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissão de novas CIN (Carteira de Identidade Nacional).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instituto de Cidadania Digital Félix Pacheco</t>
   </si>
 </sst>
 </file>
@@ -198,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -211,6 +247,10 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="20" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,7 +771,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -740,8 +780,8 @@
     <col bestFit="1" min="1" max="1" width="10.421875"/>
     <col bestFit="1" min="2" max="2" width="6.8515625"/>
     <col bestFit="1" min="3" max="3" width="12.23046875"/>
-    <col bestFit="1" min="4" max="4" width="40.57421875"/>
-    <col bestFit="1" min="5" max="5" width="22.140625"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="63.76171875"/>
+    <col bestFit="1" min="5" max="5" width="37.76171875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -997,6 +1037,96 @@
       </c>
       <c r="E15" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="2">
+        <v>45916</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="2">
+        <v>45917</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" ht="28.5">
+      <c r="A18" s="2">
+        <v>45918</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="2">
+        <v>45919</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="2">
+        <v>45918</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="2">
+        <v>45919</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>